<commit_message>
quantities now make sense (but not S < D (script 4)
</commit_message>
<xml_diff>
--- a/output/state_interviewees.xlsx
+++ b/output/state_interviewees.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -23,6 +23,9 @@
     <t xml:space="preserve">prop</t>
   </si>
   <si>
+    <t xml:space="preserve">Minas Gerais</t>
+  </si>
+  <si>
     <t xml:space="preserve">São Paulo</t>
   </si>
   <si>
@@ -56,22 +59,49 @@
     <t xml:space="preserve">Piauí</t>
   </si>
   <si>
+    <t xml:space="preserve">Goiás</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mato Grosso</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pará</t>
   </si>
   <si>
+    <t xml:space="preserve">Amazonas</t>
+  </si>
+  <si>
     <t xml:space="preserve">Alagoas</t>
   </si>
   <si>
     <t xml:space="preserve">Paraíba</t>
   </si>
   <si>
+    <t xml:space="preserve">Mato Grosso do Sul</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rio Grande do Norte</t>
   </si>
   <si>
     <t xml:space="preserve">Sergipe</t>
   </si>
   <si>
+    <t xml:space="preserve">Distrito Federal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rondônia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acre</t>
+  </si>
+  <si>
     <t xml:space="preserve">Amapá</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tocantins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roraima</t>
   </si>
   <si>
     <t xml:space="preserve">1</t>
@@ -422,10 +452,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>2923</v>
+        <v>3505</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0952086251262174</v>
+        <v>0.0797533448621098</v>
       </c>
     </row>
     <row r="3">
@@ -433,10 +463,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>2402</v>
+        <v>2923</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0782384938601348</v>
+        <v>0.0665104214071175</v>
       </c>
     </row>
     <row r="4">
@@ -444,10 +474,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>2353</v>
+        <v>2402</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0766424546431712</v>
+        <v>0.0546555019568581</v>
       </c>
     </row>
     <row r="5">
@@ -455,10 +485,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>2278</v>
+        <v>2353</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0741995374743494</v>
+        <v>0.0535405479202694</v>
       </c>
     </row>
     <row r="6">
@@ -466,10 +496,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>2063</v>
+        <v>2278</v>
       </c>
       <c r="C6" t="n">
-        <v>0.06719650825706</v>
+        <v>0.0518339856193683</v>
       </c>
     </row>
     <row r="7">
@@ -477,10 +507,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="n">
-        <v>2035</v>
+        <v>2063</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0662844858473665</v>
+        <v>0.0469418403567853</v>
       </c>
     </row>
     <row r="8">
@@ -488,10 +518,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="n">
-        <v>1997</v>
+        <v>2035</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0650467411484968</v>
+        <v>0.0463047237644489</v>
       </c>
     </row>
     <row r="9">
@@ -499,10 +529,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="n">
-        <v>1808</v>
+        <v>1997</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0588905898830657</v>
+        <v>0.0454400655319924</v>
       </c>
     </row>
     <row r="10">
@@ -510,10 +540,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="n">
-        <v>1795</v>
+        <v>1808</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0584671509071366</v>
+        <v>0.0411395285337217</v>
       </c>
     </row>
     <row r="11">
@@ -521,10 +551,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>1757</v>
+        <v>1795</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0572294062082668</v>
+        <v>0.0408437244015655</v>
       </c>
     </row>
     <row r="12">
@@ -532,10 +562,10 @@
         <v>13</v>
       </c>
       <c r="B12" t="n">
-        <v>1754</v>
+        <v>1757</v>
       </c>
       <c r="C12" t="n">
-        <v>0.057131689521514</v>
+        <v>0.0399790661691089</v>
       </c>
     </row>
     <row r="13">
@@ -543,10 +573,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="n">
-        <v>1535</v>
+        <v>1754</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0499983713885541</v>
+        <v>0.0399108036770729</v>
       </c>
     </row>
     <row r="14">
@@ -554,10 +584,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="n">
-        <v>1434</v>
+        <v>1691</v>
       </c>
       <c r="C14" t="n">
-        <v>0.046708576267874</v>
+        <v>0.038477291344316</v>
       </c>
     </row>
     <row r="15">
@@ -565,10 +595,10 @@
         <v>16</v>
       </c>
       <c r="B15" t="n">
-        <v>1425</v>
+        <v>1537</v>
       </c>
       <c r="C15" t="n">
-        <v>0.0464154262076154</v>
+        <v>0.0349731500864658</v>
       </c>
     </row>
     <row r="16">
@@ -576,10 +606,10 @@
         <v>17</v>
       </c>
       <c r="B16" t="n">
-        <v>1218</v>
+        <v>1535</v>
       </c>
       <c r="C16" t="n">
-        <v>0.039672974821667</v>
+        <v>0.0349276417584418</v>
       </c>
     </row>
     <row r="17">
@@ -587,10 +617,10 @@
         <v>18</v>
       </c>
       <c r="B17" t="n">
-        <v>1215</v>
+        <v>1500</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0395752581349142</v>
+        <v>0.0341312460180213</v>
       </c>
     </row>
     <row r="18">
@@ -598,10 +628,10 @@
         <v>19</v>
       </c>
       <c r="B18" t="n">
-        <v>709</v>
+        <v>1434</v>
       </c>
       <c r="C18" t="n">
-        <v>0.023093710302596</v>
+        <v>0.0326294711932284</v>
       </c>
     </row>
     <row r="19">
@@ -609,9 +639,119 @@
         <v>20</v>
       </c>
       <c r="B19" t="n">
-        <v>30701</v>
+        <v>1425</v>
       </c>
       <c r="C19" t="n">
+        <v>0.0324246837171202</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1287</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.0292846090834623</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="n">
+        <v>1218</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.0277145717666333</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="n">
+        <v>1215</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.0276463092745973</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="n">
+        <v>980</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.0222990807317739</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="n">
+        <v>737</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.0167698188768545</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="n">
+        <v>731</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.0166332938927824</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="n">
+        <v>709</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.0161327022845181</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" t="n">
+        <v>662</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.0150632565759534</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" t="n">
+        <v>617</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.0140393191954128</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" t="n">
+        <v>43948</v>
+      </c>
+      <c r="C29" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>